<commit_message>
Updating for Javadoc / Maven
</commit_message>
<xml_diff>
--- a/Deliverables/Project_Management/ProjectAutoAssessement.xlsx
+++ b/Deliverables/Project_Management/ProjectAutoAssessement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Studisys\OneDrive\Documents\GitHub\Lorann-Java-Project----Exia-CESI-A1\Deliverables\Project_Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0937A984-ED1A-4CBA-9770-77CF350C4EB1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B00E7C-FF7A-49C1-A4AD-B3E7AD43D6AC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{04DB42CA-C582-430A-B24B-2DA42F1F144B}"/>
   </bookViews>
@@ -772,7 +772,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -957,6 +957,16 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="25" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="25" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="25" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1667,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84878C4D-6100-4F50-9094-AD16EEDA0C55}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="94" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2132,39 +2142,39 @@
         <v>2</v>
       </c>
       <c r="L10" s="6"/>
-      <c r="M10" s="31" t="s">
+      <c r="M10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="32">
-        <v>1</v>
-      </c>
-      <c r="O10" s="33">
-        <v>1</v>
-      </c>
-      <c r="P10" s="33">
+      <c r="N10" s="20">
+        <v>1</v>
+      </c>
+      <c r="O10" s="21">
+        <v>1</v>
+      </c>
+      <c r="P10" s="21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="34">
+      <c r="Q10" s="28">
         <v>1</v>
       </c>
       <c r="S10" s="46"/>
     </row>
     <row r="11" spans="1:19" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="32">
-        <v>1</v>
-      </c>
-      <c r="C11" s="33">
-        <v>3</v>
-      </c>
-      <c r="D11" s="33">
+      <c r="B11" s="20">
+        <v>1</v>
+      </c>
+      <c r="C11" s="21">
+        <v>3</v>
+      </c>
+      <c r="D11" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="21">
         <v>1</v>
       </c>
       <c r="F11" s="6"/>
@@ -2185,20 +2195,20 @@
         <v>1</v>
       </c>
       <c r="L11" s="6"/>
-      <c r="M11" s="31" t="s">
+      <c r="M11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="32">
-        <v>1</v>
-      </c>
-      <c r="O11" s="33">
-        <v>1</v>
-      </c>
-      <c r="P11" s="33">
+      <c r="N11" s="20">
+        <v>1</v>
+      </c>
+      <c r="O11" s="21">
+        <v>1</v>
+      </c>
+      <c r="P11" s="21">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Q11" s="34">
+      <c r="Q11" s="28">
         <v>1</v>
       </c>
       <c r="S11" s="46"/>
@@ -2372,20 +2382,20 @@
       <c r="S15" s="44"/>
     </row>
     <row r="16" spans="1:19" ht="31.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="42">
-        <v>1</v>
-      </c>
-      <c r="C16" s="43">
-        <v>3</v>
-      </c>
-      <c r="D16" s="43">
+      <c r="B16" s="62">
+        <v>1</v>
+      </c>
+      <c r="C16" s="63">
+        <v>3</v>
+      </c>
+      <c r="D16" s="63">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="63">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
@@ -2405,20 +2415,20 @@
       <c r="S16" s="44"/>
     </row>
     <row r="17" spans="1:17" ht="32.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="32">
+      <c r="B17" s="38">
         <v>0</v>
       </c>
-      <c r="C17" s="33">
-        <v>1</v>
-      </c>
-      <c r="D17" s="33">
+      <c r="C17" s="39">
+        <v>1</v>
+      </c>
+      <c r="D17" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="39">
         <v>1</v>
       </c>
       <c r="F17" s="4"/>

</xml_diff>